<commit_message>
modify by hyh add field
</commit_message>
<xml_diff>
--- a/DBScript/DB scheme.xlsx
+++ b/DBScript/DB scheme.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TBL一览" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="TestResult" sheetId="6" r:id="rId6"/>
     <sheet name="TestResultDtl" sheetId="8" r:id="rId7"/>
     <sheet name="TestResultDDtl" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
   <si>
     <t>Question</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,10 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>schtime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,6 +225,22 @@
   </si>
   <si>
     <t>是否选择F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>numeric</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disorder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -327,6 +340,249 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1381125" y="352425"/>
+          <a:ext cx="990600" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>测试开始</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="342900"/>
+          <a:ext cx="990600" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>随机选题</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486399" y="342900"/>
+          <a:ext cx="1724025" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>生成</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>TestResultDtl</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="342900"/>
+          <a:ext cx="1724025" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>生成</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>TestResult</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -654,7 +910,7 @@
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -666,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E10"/>
+  <dimension ref="B3:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -696,7 +952,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -710,48 +966,57 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -765,10 +1030,13 @@
   <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="14.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:5">
       <c r="B3" s="2" t="s">
@@ -788,7 +1056,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -802,7 +1070,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -868,7 +1136,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -882,7 +1150,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -947,7 +1215,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -961,7 +1229,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -1026,7 +1294,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -1038,7 +1306,7 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -1050,19 +1318,19 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -1101,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:E12"/>
+  <dimension ref="B3:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1118,7 +1386,7 @@
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1127,7 +1395,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -1141,7 +1409,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -1155,19 +1423,19 @@
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -1179,36 +1447,46 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D9" s="1"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1220,22 +1498,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="3" spans="2:5">
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1244,7 +1522,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -1258,35 +1536,35 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -1321,4 +1599,20 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>